<commit_message>
versió final dels documents 16.06.2021
</commit_message>
<xml_diff>
--- a/k-folds aval.xlsx
+++ b/k-folds aval.xlsx
@@ -16,7 +16,6 @@
     <sheet name="poly" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -735,6 +734,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -762,27 +788,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -795,10 +800,16 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -806,18 +817,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1103,8 +1102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D5:W60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="K48" sqref="K48:K59"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W13" sqref="W13:W14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1126,11 +1125,11 @@
   <sheetData>
     <row r="5" spans="4:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="6" spans="4:23" ht="23" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="32"/>
-      <c r="E6" s="34" t="s">
+      <c r="D6" s="41"/>
+      <c r="E6" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="43" t="s">
         <v>0</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -1142,20 +1141,20 @@
       <c r="I6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="34" t="s">
+      <c r="J6" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="29" t="s">
+      <c r="K6" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="31"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="40"/>
     </row>
     <row r="7" spans="4:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D7" s="33"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
       <c r="G7" s="3" t="s">
         <v>2</v>
       </c>
@@ -1165,7 +1164,7 @@
       <c r="I7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J7" s="35"/>
+      <c r="J7" s="44"/>
       <c r="K7" s="16" t="s">
         <v>16</v>
       </c>
@@ -1180,7 +1179,7 @@
       </c>
     </row>
     <row r="8" spans="4:23" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="30" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="9">
@@ -1215,7 +1214,7 @@
       </c>
     </row>
     <row r="9" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D9" s="38"/>
+      <c r="D9" s="31"/>
       <c r="E9" s="13">
         <v>2</v>
       </c>
@@ -1248,7 +1247,7 @@
       </c>
     </row>
     <row r="10" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D10" s="38"/>
+      <c r="D10" s="31"/>
       <c r="E10" s="13">
         <v>3</v>
       </c>
@@ -1281,7 +1280,7 @@
       </c>
     </row>
     <row r="11" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D11" s="38"/>
+      <c r="D11" s="31"/>
       <c r="E11" s="13">
         <v>4</v>
       </c>
@@ -1317,7 +1316,7 @@
       </c>
     </row>
     <row r="12" spans="4:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D12" s="38"/>
+      <c r="D12" s="31"/>
       <c r="E12" s="13">
         <v>5</v>
       </c>
@@ -1359,7 +1358,7 @@
       </c>
     </row>
     <row r="13" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D13" s="38"/>
+      <c r="D13" s="31"/>
       <c r="E13" s="13">
         <v>6</v>
       </c>
@@ -1406,21 +1405,21 @@
         <f>3+8+8+10+3+10+10+11+2+22</f>
         <v>87</v>
       </c>
-      <c r="U13" s="18">
+      <c r="U13" s="26">
         <f>SUM(P13)/SUM(P13:S13)</f>
         <v>0.70068027210884354</v>
       </c>
-      <c r="V13" s="18">
+      <c r="V13" s="26">
         <f>SUM(P13:Q13)/SUM(P13:S13)</f>
         <v>0.79421768707482998</v>
       </c>
-      <c r="W13" s="36">
+      <c r="W13" s="53">
         <f>SUM(P13:Q14)/SUM(P13:S14)</f>
         <v>0.79432624113475181</v>
       </c>
     </row>
     <row r="14" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D14" s="38"/>
+      <c r="D14" s="31"/>
       <c r="E14" s="13">
         <v>7</v>
       </c>
@@ -1470,18 +1469,18 @@
         <f>1+2+1+2+1+3</f>
         <v>10</v>
       </c>
-      <c r="U14" s="18">
+      <c r="U14" s="26">
         <f>SUM(Q14)/SUM(P14:S14)</f>
         <v>0.53846153846153844</v>
       </c>
-      <c r="V14" s="18">
+      <c r="V14" s="26">
         <f>SUM(P14:Q14)/SUM(P14:S14)</f>
         <v>0.79487179487179482</v>
       </c>
-      <c r="W14" s="36"/>
+      <c r="W14" s="53"/>
     </row>
     <row r="15" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D15" s="38"/>
+      <c r="D15" s="31"/>
       <c r="E15" s="13">
         <v>8</v>
       </c>
@@ -1528,21 +1527,21 @@
         <f>0+1+2+1+2+2+2</f>
         <v>10</v>
       </c>
-      <c r="U15" s="18">
+      <c r="U15" s="26">
         <f>SUM(R15)/SUM(P15:S15)</f>
         <v>0.375</v>
       </c>
-      <c r="V15" s="18">
+      <c r="V15" s="26">
         <f>SUM(R15:S15)/SUM(P15:S15)</f>
         <v>0.5535714285714286</v>
       </c>
-      <c r="W15" s="36">
+      <c r="W15" s="53">
         <f>SUM(R15:S16)/SUM(P15:S16)</f>
         <v>0.78319783197831983</v>
       </c>
     </row>
     <row r="16" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D16" s="38"/>
+      <c r="D16" s="31"/>
       <c r="E16" s="13">
         <v>9</v>
       </c>
@@ -1589,18 +1588,18 @@
         <f>18+21+24+24+22+24+24+30+25+27</f>
         <v>239</v>
       </c>
-      <c r="U16" s="18">
+      <c r="U16" s="26">
         <f>SUM(S16)/SUM(P16:S16)</f>
         <v>0.76357827476038342</v>
       </c>
-      <c r="V16" s="18">
+      <c r="V16" s="26">
         <f>SUM(R16:S16)/SUM(P16:S16)</f>
         <v>0.82428115015974446</v>
       </c>
-      <c r="W16" s="36"/>
+      <c r="W16" s="53"/>
     </row>
     <row r="17" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D17" s="38"/>
+      <c r="D17" s="31"/>
       <c r="E17" s="13">
         <v>10</v>
       </c>
@@ -1633,7 +1632,7 @@
       </c>
     </row>
     <row r="18" spans="4:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D18" s="39"/>
+      <c r="D18" s="32"/>
       <c r="E18" s="6" t="s">
         <v>13</v>
       </c>
@@ -1674,7 +1673,7 @@
       </c>
     </row>
     <row r="19" spans="4:23" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="D19" s="37" t="s">
+      <c r="D19" s="30" t="s">
         <v>9</v>
       </c>
       <c r="E19" s="9">
@@ -1709,7 +1708,7 @@
       </c>
     </row>
     <row r="20" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D20" s="38"/>
+      <c r="D20" s="31"/>
       <c r="E20" s="13">
         <v>2</v>
       </c>
@@ -1745,7 +1744,7 @@
       </c>
     </row>
     <row r="21" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D21" s="38"/>
+      <c r="D21" s="31"/>
       <c r="E21" s="13">
         <v>3</v>
       </c>
@@ -1778,7 +1777,7 @@
       </c>
     </row>
     <row r="22" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D22" s="38"/>
+      <c r="D22" s="31"/>
       <c r="E22" s="13">
         <v>4</v>
       </c>
@@ -1836,7 +1835,7 @@
       <c r="W22" s="5"/>
     </row>
     <row r="23" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D23" s="38"/>
+      <c r="D23" s="31"/>
       <c r="E23" s="13">
         <v>5</v>
       </c>
@@ -1900,7 +1899,7 @@
       </c>
     </row>
     <row r="24" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D24" s="38"/>
+      <c r="D24" s="31"/>
       <c r="E24" s="13">
         <v>6</v>
       </c>
@@ -1958,7 +1957,7 @@
       <c r="W24" s="5"/>
     </row>
     <row r="25" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D25" s="38"/>
+      <c r="D25" s="31"/>
       <c r="E25" s="13">
         <v>7</v>
       </c>
@@ -2019,7 +2018,7 @@
       </c>
     </row>
     <row r="26" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D26" s="38"/>
+      <c r="D26" s="31"/>
       <c r="E26" s="13">
         <v>8</v>
       </c>
@@ -2055,7 +2054,7 @@
       <c r="W26" s="5"/>
     </row>
     <row r="27" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D27" s="38"/>
+      <c r="D27" s="31"/>
       <c r="E27" s="13">
         <v>9</v>
       </c>
@@ -2091,7 +2090,7 @@
       <c r="W27" s="5"/>
     </row>
     <row r="28" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D28" s="38"/>
+      <c r="D28" s="31"/>
       <c r="E28" s="13">
         <v>10</v>
       </c>
@@ -2127,7 +2126,7 @@
       <c r="W28" s="5"/>
     </row>
     <row r="29" spans="4:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D29" s="39"/>
+      <c r="D29" s="32"/>
       <c r="E29" s="6" t="s">
         <v>13</v>
       </c>
@@ -2171,7 +2170,7 @@
       <c r="W29" s="5"/>
     </row>
     <row r="30" spans="4:23" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="D30" s="40" t="s">
+      <c r="D30" s="33" t="s">
         <v>14</v>
       </c>
       <c r="E30" s="9">
@@ -2209,7 +2208,7 @@
       <c r="W30" s="5"/>
     </row>
     <row r="31" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D31" s="41"/>
+      <c r="D31" s="34"/>
       <c r="E31" s="13">
         <v>2</v>
       </c>
@@ -2245,7 +2244,7 @@
       <c r="W31" s="5"/>
     </row>
     <row r="32" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D32" s="41"/>
+      <c r="D32" s="34"/>
       <c r="E32" s="13">
         <v>3</v>
       </c>
@@ -2284,7 +2283,7 @@
       <c r="W32" s="5"/>
     </row>
     <row r="33" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D33" s="41"/>
+      <c r="D33" s="34"/>
       <c r="E33" s="13">
         <v>4</v>
       </c>
@@ -2320,7 +2319,7 @@
       <c r="W33" s="5"/>
     </row>
     <row r="34" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D34" s="41"/>
+      <c r="D34" s="34"/>
       <c r="E34" s="13">
         <v>5</v>
       </c>
@@ -2378,7 +2377,7 @@
       <c r="W34" s="5"/>
     </row>
     <row r="35" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D35" s="41"/>
+      <c r="D35" s="34"/>
       <c r="E35" s="13">
         <v>6</v>
       </c>
@@ -2442,7 +2441,7 @@
       </c>
     </row>
     <row r="36" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D36" s="41"/>
+      <c r="D36" s="34"/>
       <c r="E36" s="13">
         <v>7</v>
       </c>
@@ -2500,7 +2499,7 @@
       <c r="W36" s="5"/>
     </row>
     <row r="37" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D37" s="41"/>
+      <c r="D37" s="34"/>
       <c r="E37" s="13">
         <v>8</v>
       </c>
@@ -2561,7 +2560,7 @@
       </c>
     </row>
     <row r="38" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D38" s="41"/>
+      <c r="D38" s="34"/>
       <c r="E38" s="13">
         <v>9</v>
       </c>
@@ -2594,7 +2593,7 @@
       </c>
     </row>
     <row r="39" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D39" s="41"/>
+      <c r="D39" s="34"/>
       <c r="E39" s="13">
         <v>10</v>
       </c>
@@ -2627,7 +2626,7 @@
       </c>
     </row>
     <row r="40" spans="4:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D40" s="42"/>
+      <c r="D40" s="35"/>
       <c r="E40" s="6" t="s">
         <v>13</v>
       </c>
@@ -2684,7 +2683,7 @@
       </c>
     </row>
     <row r="48" spans="4:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G48" s="43" t="s">
+      <c r="G48" s="45" t="s">
         <v>24</v>
       </c>
       <c r="H48" s="23">
@@ -2693,52 +2692,52 @@
       <c r="I48" s="23">
         <v>0.79421768707482998</v>
       </c>
-      <c r="J48" s="46">
+      <c r="J48" s="48">
         <v>0.79432624113475181</v>
       </c>
-      <c r="K48" s="27">
+      <c r="K48" s="36">
         <f>AVERAGE(J48:J51)</f>
         <v>0.78876203655653576</v>
       </c>
     </row>
     <row r="49" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="G49" s="44"/>
+      <c r="G49" s="46"/>
       <c r="H49" s="24">
         <v>0.53846153846153844</v>
       </c>
       <c r="I49" s="24">
         <v>0.79487179487179482</v>
       </c>
-      <c r="J49" s="47"/>
-      <c r="K49" s="28"/>
+      <c r="J49" s="27"/>
+      <c r="K49" s="37"/>
     </row>
     <row r="50" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F50" s="21"/>
-      <c r="G50" s="44"/>
+      <c r="G50" s="46"/>
       <c r="H50" s="24">
         <v>0.375</v>
       </c>
       <c r="I50" s="24">
         <v>0.5535714285714286</v>
       </c>
-      <c r="J50" s="47">
+      <c r="J50" s="27">
         <v>0.78319783197831983</v>
       </c>
-      <c r="K50" s="28"/>
+      <c r="K50" s="37"/>
     </row>
     <row r="51" spans="6:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G51" s="45"/>
+      <c r="G51" s="47"/>
       <c r="H51" s="25">
         <v>0.76357827476038342</v>
       </c>
       <c r="I51" s="25">
         <v>0.82428115015974446</v>
       </c>
-      <c r="J51" s="48"/>
-      <c r="K51" s="28"/>
+      <c r="J51" s="28"/>
+      <c r="K51" s="37"/>
     </row>
     <row r="52" spans="6:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G52" s="43" t="s">
+      <c r="G52" s="45" t="s">
         <v>9</v>
       </c>
       <c r="H52" s="23">
@@ -2747,51 +2746,51 @@
       <c r="I52" s="23">
         <v>0.89795918367346939</v>
       </c>
-      <c r="J52" s="46">
+      <c r="J52" s="48">
         <v>0.88936170212765953</v>
       </c>
-      <c r="K52" s="27">
+      <c r="K52" s="36">
         <f>AVERAGE(J52:J55)</f>
         <v>0.80375944184973758</v>
       </c>
     </row>
     <row r="53" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="G53" s="44"/>
+      <c r="G53" s="46"/>
       <c r="H53" s="24">
         <v>0.47863247863247865</v>
       </c>
       <c r="I53" s="24">
         <v>0.84615384615384615</v>
       </c>
-      <c r="J53" s="47"/>
-      <c r="K53" s="28"/>
+      <c r="J53" s="27"/>
+      <c r="K53" s="37"/>
     </row>
     <row r="54" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="G54" s="44"/>
+      <c r="G54" s="46"/>
       <c r="H54" s="24">
         <v>0.32142857142857145</v>
       </c>
       <c r="I54" s="24">
         <v>0.3392857142857143</v>
       </c>
-      <c r="J54" s="47">
+      <c r="J54" s="27">
         <v>0.71815718157181574</v>
       </c>
-      <c r="K54" s="28"/>
+      <c r="K54" s="37"/>
     </row>
     <row r="55" spans="6:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G55" s="45"/>
+      <c r="G55" s="47"/>
       <c r="H55" s="25">
         <v>0.72523961661341851</v>
       </c>
       <c r="I55" s="25">
         <v>0.78594249201277955</v>
       </c>
-      <c r="J55" s="48"/>
-      <c r="K55" s="28"/>
+      <c r="J55" s="28"/>
+      <c r="K55" s="37"/>
     </row>
     <row r="56" spans="6:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G56" s="43" t="s">
+      <c r="G56" s="45" t="s">
         <v>25</v>
       </c>
       <c r="H56" s="23">
@@ -2800,48 +2799,48 @@
       <c r="I56" s="23">
         <v>0.74745762711864405</v>
       </c>
-      <c r="J56" s="46">
+      <c r="J56" s="48">
         <v>0.74857142857142855</v>
       </c>
-      <c r="K56" s="27">
+      <c r="K56" s="36">
         <f>AVERAGE(J56:J59)</f>
         <v>0.75129106187929717</v>
       </c>
     </row>
     <row r="57" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="G57" s="44"/>
+      <c r="G57" s="46"/>
       <c r="H57" s="24">
         <v>0.5</v>
       </c>
       <c r="I57" s="24">
         <v>0.75454545454545452</v>
       </c>
-      <c r="J57" s="47"/>
-      <c r="K57" s="28"/>
+      <c r="J57" s="27"/>
+      <c r="K57" s="37"/>
     </row>
     <row r="58" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="G58" s="44"/>
+      <c r="G58" s="46"/>
       <c r="H58" s="24">
         <v>0.31034482758620691</v>
       </c>
       <c r="I58" s="24">
         <v>0.5</v>
       </c>
-      <c r="J58" s="47">
+      <c r="J58" s="27">
         <v>0.75401069518716579</v>
       </c>
-      <c r="K58" s="28"/>
+      <c r="K58" s="37"/>
     </row>
     <row r="59" spans="6:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G59" s="45"/>
+      <c r="G59" s="47"/>
       <c r="H59" s="25">
         <v>0.73734177215189878</v>
       </c>
       <c r="I59" s="25">
         <v>0.80063291139240511</v>
       </c>
-      <c r="J59" s="48"/>
-      <c r="K59" s="28"/>
+      <c r="J59" s="28"/>
+      <c r="K59" s="37"/>
     </row>
     <row r="60" spans="6:11" x14ac:dyDescent="0.35">
       <c r="H60" s="18"/>
@@ -2850,12 +2849,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="J50:J51"/>
-    <mergeCell ref="W13:W14"/>
-    <mergeCell ref="W15:W16"/>
-    <mergeCell ref="D19:D29"/>
-    <mergeCell ref="D30:D40"/>
-    <mergeCell ref="D8:D18"/>
     <mergeCell ref="K56:K59"/>
     <mergeCell ref="K52:K55"/>
     <mergeCell ref="K48:K51"/>
@@ -2872,6 +2865,12 @@
     <mergeCell ref="J56:J57"/>
     <mergeCell ref="J54:J55"/>
     <mergeCell ref="J52:J53"/>
+    <mergeCell ref="J50:J51"/>
+    <mergeCell ref="W13:W14"/>
+    <mergeCell ref="W15:W16"/>
+    <mergeCell ref="D19:D29"/>
+    <mergeCell ref="D30:D40"/>
+    <mergeCell ref="D8:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2909,11 +2908,11 @@
   <sheetData>
     <row r="5" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="6" spans="2:22" ht="23" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="32"/>
-      <c r="C6" s="34" t="s">
+      <c r="B6" s="41"/>
+      <c r="C6" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="43" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -2925,20 +2924,20 @@
       <c r="G6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="34" t="s">
+      <c r="H6" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="29" t="s">
+      <c r="I6" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="31"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="40"/>
     </row>
     <row r="7" spans="2:22" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="33"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
       <c r="E7" s="3" t="s">
         <v>2</v>
       </c>
@@ -2948,7 +2947,7 @@
       <c r="G7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="35"/>
+      <c r="H7" s="44"/>
       <c r="I7" s="16" t="s">
         <v>16</v>
       </c>
@@ -2963,7 +2962,7 @@
       </c>
     </row>
     <row r="8" spans="2:22" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="30" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="9">
@@ -2998,7 +2997,7 @@
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B9" s="38"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="13">
         <v>2</v>
       </c>
@@ -3031,7 +3030,7 @@
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B10" s="38"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="13">
         <v>3</v>
       </c>
@@ -3064,7 +3063,7 @@
       </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B11" s="38"/>
+      <c r="B11" s="31"/>
       <c r="C11" s="13">
         <v>4</v>
       </c>
@@ -3100,7 +3099,7 @@
       </c>
     </row>
     <row r="12" spans="2:22" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="38"/>
+      <c r="B12" s="31"/>
       <c r="C12" s="13">
         <v>5</v>
       </c>
@@ -3142,7 +3141,7 @@
       </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B13" s="38"/>
+      <c r="B13" s="31"/>
       <c r="C13" s="13">
         <v>6</v>
       </c>
@@ -3197,14 +3196,14 @@
         <f>SUM(N13:O13)/SUM(N13:Q13)</f>
         <v>0.90054054054054056</v>
       </c>
-      <c r="U13" s="49">
+      <c r="U13" s="53">
         <f>SUM(N13:O14)/SUM(N13:Q14)</f>
         <v>0.90072202166064985</v>
       </c>
-      <c r="V13" s="50"/>
+      <c r="V13" s="54"/>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B14" s="38"/>
+      <c r="B14" s="31"/>
       <c r="C14" s="13">
         <v>7</v>
       </c>
@@ -3262,11 +3261,11 @@
         <f>SUM(N14:O14)/SUM(N14:Q14)</f>
         <v>0.90163934426229508</v>
       </c>
-      <c r="U14" s="49"/>
-      <c r="V14" s="50"/>
+      <c r="U14" s="53"/>
+      <c r="V14" s="54"/>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B15" s="38"/>
+      <c r="B15" s="31"/>
       <c r="C15" s="13">
         <v>8</v>
       </c>
@@ -3321,14 +3320,14 @@
         <f>SUM(P15:Q15)/SUM(N15:Q15)</f>
         <v>0.12</v>
       </c>
-      <c r="U15" s="49">
+      <c r="U15" s="53">
         <f>SUM(P15:Q16)/SUM(N15:Q16)</f>
         <v>0.41855203619909503</v>
       </c>
-      <c r="V15" s="50"/>
+      <c r="V15" s="54"/>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B16" s="38"/>
+      <c r="B16" s="31"/>
       <c r="C16" s="13">
         <v>9</v>
       </c>
@@ -3383,11 +3382,11 @@
         <f>SUM(P16:Q16)/SUM(N16:Q16)</f>
         <v>0.47956403269754766</v>
       </c>
-      <c r="U16" s="49"/>
-      <c r="V16" s="50"/>
+      <c r="U16" s="53"/>
+      <c r="V16" s="54"/>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B17" s="38"/>
+      <c r="B17" s="31"/>
       <c r="C17" s="13">
         <v>10</v>
       </c>
@@ -3420,7 +3419,7 @@
       </c>
     </row>
     <row r="18" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="39"/>
+      <c r="B18" s="32"/>
       <c r="C18" s="6" t="s">
         <v>13</v>
       </c>
@@ -3461,7 +3460,7 @@
       </c>
     </row>
     <row r="19" spans="2:21" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="30" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="9">
@@ -3496,7 +3495,7 @@
       </c>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B20" s="38"/>
+      <c r="B20" s="31"/>
       <c r="C20" s="13">
         <v>2</v>
       </c>
@@ -3529,7 +3528,7 @@
       </c>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B21" s="38"/>
+      <c r="B21" s="31"/>
       <c r="C21" s="13">
         <v>3</v>
       </c>
@@ -3562,7 +3561,7 @@
       </c>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B22" s="38"/>
+      <c r="B22" s="31"/>
       <c r="C22" s="13">
         <v>4</v>
       </c>
@@ -3598,7 +3597,7 @@
       </c>
     </row>
     <row r="23" spans="2:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="38"/>
+      <c r="B23" s="31"/>
       <c r="C23" s="13">
         <v>5</v>
       </c>
@@ -3640,7 +3639,7 @@
       </c>
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B24" s="38"/>
+      <c r="B24" s="31"/>
       <c r="C24" s="13">
         <v>6</v>
       </c>
@@ -3695,13 +3694,13 @@
         <f>SUM(N24:O24)/SUM(N24:Q24)</f>
         <v>0.87282608695652175</v>
       </c>
-      <c r="U24" s="36">
+      <c r="U24" s="29">
         <f>SUM(N24:O25)/SUM(N24:Q25)</f>
         <v>0.87340619307832423</v>
       </c>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B25" s="38"/>
+      <c r="B25" s="31"/>
       <c r="C25" s="13">
         <v>7</v>
       </c>
@@ -3759,10 +3758,10 @@
         <f>SUM(N25:O25)/SUM(N25:Q25)</f>
         <v>0.8764044943820225</v>
       </c>
-      <c r="U25" s="36"/>
+      <c r="U25" s="29"/>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B26" s="38"/>
+      <c r="B26" s="31"/>
       <c r="C26" s="13">
         <v>8</v>
       </c>
@@ -3817,13 +3816,13 @@
         <f>SUM(P26:Q26)/SUM(N26:Q26)</f>
         <v>0.34</v>
       </c>
-      <c r="U26" s="36">
+      <c r="U26" s="29">
         <f>SUM(P26:Q27)/SUM(N26:Q27)</f>
         <v>0.66371681415929207</v>
       </c>
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B27" s="38"/>
+      <c r="B27" s="31"/>
       <c r="C27" s="13">
         <v>9</v>
       </c>
@@ -3878,10 +3877,10 @@
         <f>SUM(P27:Q27)/SUM(N27:Q27)</f>
         <v>0.70398009950248752</v>
       </c>
-      <c r="U27" s="36"/>
+      <c r="U27" s="29"/>
     </row>
     <row r="28" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B28" s="38"/>
+      <c r="B28" s="31"/>
       <c r="C28" s="13">
         <v>10</v>
       </c>
@@ -3914,7 +3913,7 @@
       </c>
     </row>
     <row r="29" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="39"/>
+      <c r="B29" s="32"/>
       <c r="C29" s="6" t="s">
         <v>13</v>
       </c>
@@ -3955,7 +3954,7 @@
       </c>
     </row>
     <row r="30" spans="2:21" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="37" t="s">
+      <c r="B30" s="30" t="s">
         <v>27</v>
       </c>
       <c r="C30" s="9">
@@ -3990,7 +3989,7 @@
       </c>
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B31" s="38"/>
+      <c r="B31" s="31"/>
       <c r="C31" s="13">
         <v>2</v>
       </c>
@@ -4026,7 +4025,7 @@
       </c>
     </row>
     <row r="32" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B32" s="38"/>
+      <c r="B32" s="31"/>
       <c r="C32" s="13">
         <v>3</v>
       </c>
@@ -4059,7 +4058,7 @@
       </c>
     </row>
     <row r="33" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B33" s="38"/>
+      <c r="B33" s="31"/>
       <c r="C33" s="13">
         <v>4</v>
       </c>
@@ -4114,13 +4113,13 @@
         <f>SUM(N33:O33)/SUM(N33:Q33)</f>
         <v>0.84565217391304348</v>
       </c>
-      <c r="U33" s="36">
+      <c r="U33" s="29">
         <f>SUM(N33:O34)/SUM(N33:Q34)</f>
         <v>0.83894449499545043</v>
       </c>
     </row>
     <row r="34" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B34" s="38"/>
+      <c r="B34" s="31"/>
       <c r="C34" s="13">
         <v>5</v>
       </c>
@@ -4178,10 +4177,10 @@
         <f>SUM(N34:O34)/SUM(N34:Q34)</f>
         <v>0.8044692737430168</v>
       </c>
-      <c r="U34" s="36"/>
+      <c r="U34" s="29"/>
     </row>
     <row r="35" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B35" s="38"/>
+      <c r="B35" s="31"/>
       <c r="C35" s="13">
         <v>6</v>
       </c>
@@ -4236,13 +4235,13 @@
         <f>SUM(P35:Q35)/SUM(N35:Q35)</f>
         <v>0.41666666666666669</v>
       </c>
-      <c r="U35" s="36">
+      <c r="U35" s="29">
         <f>SUM(P35:Q36)/SUM(N35:Q36)</f>
         <v>0.7117516629711752</v>
       </c>
     </row>
     <row r="36" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B36" s="38"/>
+      <c r="B36" s="31"/>
       <c r="C36" s="13">
         <v>7</v>
       </c>
@@ -4297,10 +4296,10 @@
         <f>SUM(P36:Q36)/SUM(N36:Q36)</f>
         <v>0.74689826302729534</v>
       </c>
-      <c r="U36" s="36"/>
+      <c r="U36" s="29"/>
     </row>
     <row r="37" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B37" s="38"/>
+      <c r="B37" s="31"/>
       <c r="C37" s="13">
         <v>8</v>
       </c>
@@ -4336,7 +4335,7 @@
       <c r="U37" s="5"/>
     </row>
     <row r="38" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B38" s="38"/>
+      <c r="B38" s="31"/>
       <c r="C38" s="13">
         <v>9</v>
       </c>
@@ -4372,7 +4371,7 @@
       <c r="U38" s="5"/>
     </row>
     <row r="39" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B39" s="38"/>
+      <c r="B39" s="31"/>
       <c r="C39" s="13">
         <v>10</v>
       </c>
@@ -4408,7 +4407,7 @@
       <c r="U39" s="5"/>
     </row>
     <row r="40" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B40" s="39"/>
+      <c r="B40" s="32"/>
       <c r="C40" s="6" t="s">
         <v>13</v>
       </c>
@@ -4468,7 +4467,7 @@
       </c>
     </row>
     <row r="48" spans="2:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E48" s="43" t="s">
+      <c r="E48" s="45" t="s">
         <v>31</v>
       </c>
       <c r="F48" s="23">
@@ -4477,51 +4476,51 @@
       <c r="G48" s="23">
         <v>0.90054054054054056</v>
       </c>
-      <c r="H48" s="51">
+      <c r="H48" s="49">
         <v>0.90072202166064985</v>
       </c>
-      <c r="I48" s="27">
+      <c r="I48" s="36">
         <f>AVERAGE(H48:H51)</f>
         <v>0.65963702892987242</v>
       </c>
     </row>
     <row r="49" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="E49" s="44"/>
+      <c r="E49" s="46"/>
       <c r="F49" s="24">
         <v>0.3551912568306011</v>
       </c>
       <c r="G49" s="24">
         <v>0.90163934426229508</v>
       </c>
-      <c r="H49" s="52"/>
-      <c r="I49" s="28"/>
+      <c r="H49" s="50"/>
+      <c r="I49" s="37"/>
     </row>
     <row r="50" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="E50" s="44"/>
+      <c r="E50" s="46"/>
       <c r="F50" s="24">
         <v>1.3333333333333334E-2</v>
       </c>
       <c r="G50" s="24">
         <v>0.12</v>
       </c>
-      <c r="H50" s="53">
+      <c r="H50" s="51">
         <v>0.41855203619909503</v>
       </c>
-      <c r="I50" s="28"/>
+      <c r="I50" s="37"/>
     </row>
     <row r="51" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E51" s="45"/>
+      <c r="E51" s="47"/>
       <c r="F51" s="25">
         <v>0.47411444141689374</v>
       </c>
       <c r="G51" s="25">
         <v>0.47956403269754766</v>
       </c>
-      <c r="H51" s="54"/>
-      <c r="I51" s="28"/>
+      <c r="H51" s="52"/>
+      <c r="I51" s="37"/>
     </row>
     <row r="52" spans="4:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E52" s="43" t="s">
+      <c r="E52" s="45" t="s">
         <v>28</v>
       </c>
       <c r="F52" s="23">
@@ -4530,52 +4529,52 @@
       <c r="G52" s="23">
         <v>0.87282608695652175</v>
       </c>
-      <c r="H52" s="51">
+      <c r="H52" s="49">
         <v>0.87340619307832423</v>
       </c>
-      <c r="I52" s="27">
+      <c r="I52" s="36">
         <f>AVERAGE(H52:H55)</f>
         <v>0.76856150361880815</v>
       </c>
     </row>
     <row r="53" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="E53" s="44"/>
+      <c r="E53" s="46"/>
       <c r="F53" s="24">
         <v>0.37640449438202245</v>
       </c>
       <c r="G53" s="24">
         <v>0.8764044943820225</v>
       </c>
-      <c r="H53" s="52"/>
-      <c r="I53" s="28"/>
+      <c r="H53" s="50"/>
+      <c r="I53" s="37"/>
     </row>
     <row r="54" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D54" s="21"/>
-      <c r="E54" s="44"/>
+      <c r="E54" s="46"/>
       <c r="F54" s="24">
         <v>0.02</v>
       </c>
       <c r="G54" s="24">
         <v>0.34</v>
       </c>
-      <c r="H54" s="53">
+      <c r="H54" s="51">
         <v>0.66371681415929207</v>
       </c>
-      <c r="I54" s="28"/>
+      <c r="I54" s="37"/>
     </row>
     <row r="55" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E55" s="45"/>
+      <c r="E55" s="47"/>
       <c r="F55" s="25">
         <v>0.69900497512437809</v>
       </c>
       <c r="G55" s="25">
         <v>0.70398009950248752</v>
       </c>
-      <c r="H55" s="54"/>
-      <c r="I55" s="28"/>
+      <c r="H55" s="52"/>
+      <c r="I55" s="37"/>
     </row>
     <row r="56" spans="4:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E56" s="43" t="s">
+      <c r="E56" s="45" t="s">
         <v>29</v>
       </c>
       <c r="F56" s="23">
@@ -4584,78 +4583,78 @@
       <c r="G56" s="23">
         <v>0.84565217391304348</v>
       </c>
-      <c r="H56" s="51">
+      <c r="H56" s="49">
         <v>0.83894449499545043</v>
       </c>
-      <c r="I56" s="27">
+      <c r="I56" s="36">
         <f>AVERAGE(H56:H59)</f>
         <v>0.77534807898331282</v>
       </c>
     </row>
     <row r="57" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="E57" s="44"/>
+      <c r="E57" s="46"/>
       <c r="F57" s="24">
         <v>0.40782122905027934</v>
       </c>
       <c r="G57" s="24">
         <v>0.8044692737430168</v>
       </c>
-      <c r="H57" s="52"/>
-      <c r="I57" s="28"/>
+      <c r="H57" s="50"/>
+      <c r="I57" s="37"/>
     </row>
     <row r="58" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="E58" s="44"/>
+      <c r="E58" s="46"/>
       <c r="F58" s="24">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G58" s="24">
         <v>0.41666666666666669</v>
       </c>
-      <c r="H58" s="53">
+      <c r="H58" s="51">
         <v>0.7117516629711752</v>
       </c>
-      <c r="I58" s="28"/>
+      <c r="I58" s="37"/>
     </row>
     <row r="59" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E59" s="45"/>
+      <c r="E59" s="47"/>
       <c r="F59" s="25">
         <v>0.74193548387096775</v>
       </c>
       <c r="G59" s="25">
         <v>0.74689826302729534</v>
       </c>
-      <c r="H59" s="54"/>
-      <c r="I59" s="28"/>
+      <c r="H59" s="52"/>
+      <c r="I59" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B19:B29"/>
-    <mergeCell ref="B8:B18"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E56:E59"/>
+    <mergeCell ref="H56:H57"/>
+    <mergeCell ref="H58:H59"/>
+    <mergeCell ref="U24:U25"/>
+    <mergeCell ref="U26:U27"/>
+    <mergeCell ref="V13:V16"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="H48:H49"/>
+    <mergeCell ref="H50:H51"/>
+    <mergeCell ref="I48:I51"/>
+    <mergeCell ref="U33:U34"/>
+    <mergeCell ref="U35:U36"/>
+    <mergeCell ref="I52:I55"/>
+    <mergeCell ref="I56:I59"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="U15:U16"/>
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="I6:L6"/>
     <mergeCell ref="B30:B40"/>
     <mergeCell ref="E52:E55"/>
     <mergeCell ref="H52:H53"/>
     <mergeCell ref="H54:H55"/>
-    <mergeCell ref="U33:U34"/>
-    <mergeCell ref="U35:U36"/>
-    <mergeCell ref="I52:I55"/>
-    <mergeCell ref="I56:I59"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="U15:U16"/>
-    <mergeCell ref="V13:V16"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="H48:H49"/>
-    <mergeCell ref="H50:H51"/>
-    <mergeCell ref="I48:I51"/>
-    <mergeCell ref="E56:E59"/>
-    <mergeCell ref="H56:H57"/>
-    <mergeCell ref="H58:H59"/>
-    <mergeCell ref="U24:U25"/>
-    <mergeCell ref="U26:U27"/>
+    <mergeCell ref="B19:B29"/>
+    <mergeCell ref="B8:B18"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>